<commit_message>
fix celery and analytics
</commit_message>
<xml_diff>
--- a/app/api/management/commands/JUQSDR_Tutorial_1-results.xlsx
+++ b/app/api/management/commands/JUQSDR_Tutorial_1-results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8758032-6CFB-4E95-8232-E9F775B4FE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741E884D-44F3-4F26-967A-80D1A9AC2090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22395" yWindow="3315" windowWidth="23640" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main results" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="188">
   <si>
     <t>#</t>
   </si>
@@ -589,16 +589,36 @@
   </si>
   <si>
     <t>Archived?</t>
+  </si>
+  <si>
+    <t>TEOH XI SHENG</t>
+  </si>
+  <si>
+    <t>XI SHENG</t>
+  </si>
+  <si>
+    <t>TEOH</t>
+  </si>
+  <si>
+    <t>c210101@e.ntu.edu.sg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -621,16 +641,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -968,11 +993,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
@@ -986,7 +1013,7 @@
     <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1056,7 +1083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1091,7 +1118,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1126,7 +1153,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1161,7 +1188,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1196,7 +1223,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1231,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1266,7 +1293,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1301,7 +1328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1336,7 +1363,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1371,7 +1398,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1406,7 +1433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1441,7 +1468,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1476,7 +1503,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1511,7 +1538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1546,7 +1573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1581,7 +1608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1616,7 +1643,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1651,7 +1678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1686,7 +1713,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1721,42 +1748,80 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{274466CD-FBB6-4A4C-B66C-520C0AB707D3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
@@ -1768,7 +1833,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1776,7 +1841,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -1784,7 +1849,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>131</v>
       </c>
@@ -1798,7 +1863,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -1812,7 +1877,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>136</v>
       </c>
@@ -1826,7 +1891,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>137</v>
       </c>
@@ -1840,7 +1905,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
@@ -1854,7 +1919,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
@@ -1866,7 +1931,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -1878,7 +1943,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>141</v>
       </c>
@@ -1890,7 +1955,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>142</v>
       </c>
@@ -1902,7 +1967,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
@@ -1914,7 +1979,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -1926,7 +1991,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
@@ -1938,7 +2003,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>146</v>
       </c>
@@ -1948,7 +2013,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>147</v>
       </c>
@@ -1970,7 +2035,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1978,7 +2043,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -1986,7 +2051,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>131</v>
       </c>
@@ -2000,7 +2065,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
@@ -2014,7 +2079,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
@@ -2028,7 +2093,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>151</v>
       </c>
@@ -2042,7 +2107,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>152</v>
       </c>
@@ -2056,7 +2121,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>153</v>
       </c>
@@ -2070,7 +2135,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>154</v>
       </c>
@@ -2084,7 +2149,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>155</v>
       </c>
@@ -2098,7 +2163,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>139</v>
       </c>
@@ -2110,7 +2175,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>140</v>
       </c>
@@ -2122,7 +2187,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
@@ -2134,7 +2199,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>142</v>
       </c>
@@ -2146,7 +2211,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>143</v>
       </c>
@@ -2158,7 +2223,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>144</v>
       </c>
@@ -2170,7 +2235,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>145</v>
       </c>
@@ -2182,7 +2247,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>146</v>
       </c>
@@ -2192,7 +2257,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>147</v>
       </c>
@@ -2214,7 +2279,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -2222,7 +2287,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
@@ -2230,7 +2295,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>131</v>
       </c>
@@ -2244,7 +2309,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>158</v>
       </c>
@@ -2258,7 +2323,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>159</v>
       </c>
@@ -2272,7 +2337,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
@@ -2286,7 +2351,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>161</v>
       </c>
@@ -2300,7 +2365,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
@@ -2312,7 +2377,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -2324,7 +2389,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>141</v>
       </c>
@@ -2336,7 +2401,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>142</v>
       </c>
@@ -2348,7 +2413,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
@@ -2360,7 +2425,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -2372,7 +2437,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
@@ -2384,7 +2449,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>146</v>
       </c>
@@ -2394,7 +2459,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>147</v>
       </c>
@@ -2416,7 +2481,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -2424,7 +2489,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>162</v>
       </c>
@@ -2432,7 +2497,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>131</v>
       </c>
@@ -2446,7 +2511,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>163</v>
       </c>
@@ -2460,7 +2525,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>164</v>
       </c>
@@ -2474,7 +2539,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>165</v>
       </c>
@@ -2488,7 +2553,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>166</v>
       </c>
@@ -2502,7 +2567,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
@@ -2514,7 +2579,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -2526,7 +2591,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>141</v>
       </c>
@@ -2538,7 +2603,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>142</v>
       </c>
@@ -2550,7 +2615,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
@@ -2562,7 +2627,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -2574,7 +2639,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
@@ -2586,7 +2651,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>146</v>
       </c>
@@ -2596,7 +2661,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>147</v>
       </c>
@@ -2618,181 +2683,181 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>181</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>139</v>
       </c>
@@ -2803,7 +2868,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>140</v>
       </c>
@@ -2814,7 +2879,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>141</v>
       </c>
@@ -2825,7 +2890,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>142</v>
       </c>
@@ -2836,7 +2901,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>143</v>
       </c>
@@ -2847,7 +2912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>144</v>
       </c>
@@ -2858,7 +2923,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>145</v>
       </c>
@@ -2869,7 +2934,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>146</v>
       </c>
@@ -2878,7 +2943,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>147</v>
       </c>
@@ -2899,7 +2964,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -2909,7 +2974,7 @@
     <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2930,7 +2995,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>146</v>
       </c>
@@ -2943,7 +3008,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>147</v>
       </c>

</xml_diff>